<commit_message>
bug fixes on test 5 generator
</commit_message>
<xml_diff>
--- a/group-reports/tables/shahriar-1-2-tests-first-results.xlsx
+++ b/group-reports/tables/shahriar-1-2-tests-first-results.xlsx
@@ -722,12 +722,12 @@
       </c>
       <c r="O3" s="1" t="inlineStr">
         <is>
-          <t>644</t>
+          <t>1839</t>
         </is>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
-          <t>12283k</t>
+          <t>12516k</t>
         </is>
       </c>
       <c r="Q3" s="1" t="inlineStr">
@@ -844,12 +844,12 @@
       </c>
       <c r="O4" s="1" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>1806</t>
         </is>
       </c>
       <c r="P4" s="1" t="inlineStr">
         <is>
-          <t>5228.2k</t>
+          <t>6480.3k</t>
         </is>
       </c>
       <c r="Q4" s="1" t="inlineStr">
@@ -966,12 +966,12 @@
       </c>
       <c r="O5" s="1" t="inlineStr">
         <is>
-          <t>1827</t>
+          <t>1361</t>
         </is>
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
-          <t>8409.4k</t>
+          <t>8460.8k</t>
         </is>
       </c>
       <c r="Q5" s="1" t="inlineStr">
@@ -1088,12 +1088,12 @@
       </c>
       <c r="O6" s="1" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
-          <t>5207.8k</t>
+          <t>6680</t>
         </is>
       </c>
       <c r="Q6" s="1" t="inlineStr">
@@ -1210,12 +1210,12 @@
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1775</t>
         </is>
       </c>
       <c r="P7" s="1" t="inlineStr">
         <is>
-          <t>3174</t>
+          <t>1696.7k</t>
         </is>
       </c>
       <c r="Q7" s="1" t="inlineStr">
@@ -1332,12 +1332,12 @@
       </c>
       <c r="O8" s="1" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>1615</t>
         </is>
       </c>
       <c r="P8" s="1" t="inlineStr">
         <is>
-          <t>2414</t>
+          <t>1079.8k</t>
         </is>
       </c>
       <c r="Q8" s="1" t="inlineStr">
@@ -1454,12 +1454,12 @@
       </c>
       <c r="O9" s="1" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P9" s="1" t="inlineStr">
         <is>
-          <t>2643</t>
+          <t>2396</t>
         </is>
       </c>
       <c r="Q9" s="1" t="inlineStr">
@@ -1576,12 +1576,12 @@
       </c>
       <c r="O10" s="1" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
-          <t>5010.5k</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="Q10" s="1" t="inlineStr">
@@ -1698,12 +1698,12 @@
       </c>
       <c r="O11" s="1" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>1907</t>
         </is>
       </c>
       <c r="P11" s="1" t="inlineStr">
         <is>
-          <t>2824</t>
+          <t>1807.9k</t>
         </is>
       </c>
       <c r="Q11" s="1" t="inlineStr">
@@ -1820,12 +1820,12 @@
       </c>
       <c r="O12" s="1" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P12" s="1" t="inlineStr">
         <is>
-          <t>2705</t>
+          <t>1280</t>
         </is>
       </c>
       <c r="Q12" s="1" t="inlineStr">
@@ -1942,12 +1942,12 @@
       </c>
       <c r="O13" s="1" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>1860</t>
         </is>
       </c>
       <c r="P13" s="1" t="inlineStr">
         <is>
-          <t>5199.3k</t>
+          <t>6696.6k</t>
         </is>
       </c>
       <c r="Q13" s="1" t="inlineStr">
@@ -2064,12 +2064,12 @@
       </c>
       <c r="O14" s="1" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1888</t>
         </is>
       </c>
       <c r="P14" s="1" t="inlineStr">
         <is>
-          <t>2693</t>
+          <t>2682.8k</t>
         </is>
       </c>
       <c r="Q14" s="1" t="inlineStr">
@@ -2186,12 +2186,12 @@
       </c>
       <c r="O15" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>1337</t>
         </is>
       </c>
       <c r="P15" s="1" t="inlineStr">
         <is>
-          <t>2617</t>
+          <t>3111.3k</t>
         </is>
       </c>
       <c r="Q15" s="1" t="inlineStr">

</xml_diff>

<commit_message>
bug fixes on repost test 5
</commit_message>
<xml_diff>
--- a/group-reports/tables/shahriar-1-2-tests-first-results.xlsx
+++ b/group-reports/tables/shahriar-1-2-tests-first-results.xlsx
@@ -732,7 +732,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>1222478.70</t>
+          <t>942546.03</t>
         </is>
       </c>
       <c r="R3" s="1" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="Q4" s="1" t="inlineStr">
         <is>
-          <t>718579.80</t>
+          <t>1856615.58</t>
         </is>
       </c>
       <c r="R4" s="1" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="Q5" s="1" t="inlineStr">
         <is>
-          <t>1248472.63</t>
+          <t>103743.50</t>
         </is>
       </c>
       <c r="R5" s="1" t="inlineStr">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="Q6" s="1" t="inlineStr">
         <is>
-          <t>719239.21</t>
+          <t>1870.33</t>
         </is>
       </c>
       <c r="R6" s="1" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="Q7" s="1" t="inlineStr">
         <is>
-          <t>1276.35</t>
+          <t>6417.59</t>
         </is>
       </c>
       <c r="R7" s="1" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="Q8" s="1" t="inlineStr">
         <is>
-          <t>1276.09</t>
+          <t>6875.05</t>
         </is>
       </c>
       <c r="R8" s="1" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="Q9" s="1" t="inlineStr">
         <is>
-          <t>1271.05</t>
+          <t>19.15</t>
         </is>
       </c>
       <c r="R9" s="1" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="Q10" s="1" t="inlineStr">
         <is>
-          <t>989279.56</t>
+          <t>971.99</t>
         </is>
       </c>
       <c r="R10" s="1" t="inlineStr">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="Q11" s="1" t="inlineStr">
         <is>
-          <t>1273.74</t>
+          <t>12720.64</t>
         </is>
       </c>
       <c r="R11" s="1" t="inlineStr">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="Q12" s="1" t="inlineStr">
         <is>
-          <t>1271.44</t>
+          <t>17.60</t>
         </is>
       </c>
       <c r="R12" s="1" t="inlineStr">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="Q13" s="1" t="inlineStr">
         <is>
-          <t>763255.80</t>
+          <t>1669827.70</t>
         </is>
       </c>
       <c r="R13" s="1" t="inlineStr">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="Q14" s="1" t="inlineStr">
         <is>
-          <t>1272.23</t>
+          <t>15779.13</t>
         </is>
       </c>
       <c r="R14" s="1" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="Q15" s="1" t="inlineStr">
         <is>
-          <t>1220.28</t>
+          <t>137542.26</t>
         </is>
       </c>
       <c r="R15" s="1" t="inlineStr">

</xml_diff>